<commit_message>
Uptadet verion of transformar calculation
</commit_message>
<xml_diff>
--- a/Flyback_converter_AB/Transformer_Design.xlsx
+++ b/Flyback_converter_AB/Transformer_Design.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ali Belli\Documents\EE464_term_project_Social_Isolation\Flyback_converter_AB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/87011da2d366edf5/Belgeler/EE464_term_project_Social_Isiolation/Flyback_converter_AB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB78AAE-B3F2-4BA0-97FA-A65965CC0F00}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{6AB78AAE-B3F2-4BA0-97FA-A65965CC0F00}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{975CB990-5AD8-4A67-813B-852773F220E9}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="63">
   <si>
     <t>Desired Output Voltage Ripple(%)</t>
   </si>
@@ -314,6 +314,56 @@
   <si>
     <t>Secondary Resistance(mohm)</t>
   </si>
+  <si>
+    <t>Secondary Inductance(µH)</t>
+  </si>
+  <si>
+    <r>
+      <t>Primary Inductance(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial Tur"/>
+        <charset val="162"/>
+      </rPr>
+      <t>µ</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="162"/>
+      </rPr>
+      <t>H</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="162"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Effective magnetic path length (mm)</t>
+  </si>
+  <si>
+    <t>Relative permeability of core material</t>
+  </si>
+  <si>
+    <t>Airgap (mm)</t>
+  </si>
 </sst>
 </file>
 
@@ -323,12 +373,20 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -399,14 +457,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -415,7 +473,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -424,11 +482,14 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -709,25 +770,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="2"/>
-    <col min="3" max="3" width="3.140625" customWidth="1"/>
-    <col min="4" max="4" width="42.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="2"/>
-    <col min="6" max="6" width="2.85546875" customWidth="1"/>
-    <col min="7" max="7" width="44.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="34.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" style="2"/>
+    <col min="3" max="3" width="3.109375" customWidth="1"/>
+    <col min="4" max="4" width="42.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="2"/>
+    <col min="6" max="6" width="2.88671875" customWidth="1"/>
+    <col min="7" max="7" width="44.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
@@ -747,7 +808,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -759,7 +820,7 @@
       </c>
       <c r="E2" s="6">
         <f>(B4+B6)*(1-B7/100)/(B12*1000)/(B16)/(B9/100)*1000000</f>
-        <v>3.5999999999999992</v>
+        <v>4.2249999999999996</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>36</v>
@@ -768,7 +829,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -780,7 +841,7 @@
       </c>
       <c r="E3" s="6">
         <f>E2*B18^2</f>
-        <v>435.59999999999991</v>
+        <v>342.22499999999997</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>38</v>
@@ -789,7 +850,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -801,7 +862,7 @@
       </c>
       <c r="E4" s="5">
         <f>(B4+B6)*(1-B20)/(B12*1000)/(B16)/(B9/100)*1000000</f>
-        <v>3.7499999999999996</v>
+        <v>4.3597560975609753</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>37</v>
@@ -810,7 +871,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -822,7 +883,7 @@
       </c>
       <c r="E5" s="5">
         <f>E4*E26^2</f>
-        <v>320.85937499999994</v>
+        <v>302.76084010840111</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>39</v>
@@ -831,7 +892,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -843,29 +904,29 @@
       </c>
       <c r="E6" s="5">
         <f>(B4+B6)*(1-B22)/(B12*1000)/(B16)/(B9/100)*1000000</f>
-        <v>3.9879154078549841</v>
+        <v>4.4687499999999991</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>40</v>
       </c>
       <c r="H6" s="9">
         <f>(1-B22)/(B5/B4)*0.05*E26*B11*10</f>
-        <v>29.510574018126889</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>27.499999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="5">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>53</v>
       </c>
       <c r="E7" s="5">
         <f>E6*E26^2</f>
-        <v>341.21601208459208</v>
+        <v>310.32986111111109</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>42</v>
@@ -874,7 +935,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>0</v>
       </c>
@@ -884,7 +945,7 @@
       <c r="D8" s="10"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
@@ -892,7 +953,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
@@ -910,7 +971,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
@@ -928,10 +989,10 @@
       </c>
       <c r="H11" s="8">
         <f>0.8*(B4+B6)*E26*H7/1000/(H5/H6)</f>
-        <v>1.3648640483383685</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1.1458333333333333</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
@@ -942,47 +1003,51 @@
         <v>28</v>
       </c>
       <c r="E12" s="5">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>44</v>
       </c>
       <c r="H12" s="8">
-        <f>(2*(B4+B6)*B16*(1+B9/100))/B11*100/(H5/H6)^2/B12</f>
-        <v>0.50397799703665846</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <f>(2*(B4+B6)*B5/B4)/B11*100/(H5/H6)^2/B12</f>
+        <v>0.13129340277777776</v>
+      </c>
+      <c r="I12">
+        <f>B16*(1+B9/100)</f>
+        <v>25.641025641025642</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D13" s="3" t="s">
         <v>49</v>
       </c>
       <c r="E13" s="5">
-        <v>192</v>
+        <v>120</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>45</v>
       </c>
       <c r="H13" s="8">
         <f>H4*B2/(H3/H6)/1000000</f>
-        <v>0.17706344410876132</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.16499999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D14" s="3" t="s">
         <v>47</v>
       </c>
       <c r="E14" s="5">
-        <v>454</v>
+        <v>621</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>46</v>
       </c>
       <c r="H14" s="8">
         <f>H2*E26*(B4+B6)/(H3/H6)/1000000</f>
-        <v>0.13648640483383687</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.11458333333333333</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -998,30 +1063,35 @@
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="6">
         <f>B5/B4/(1-B7/100)</f>
-        <v>13.888888888888891</v>
-      </c>
-      <c r="E16" s="10"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>12.820512820512821</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="13">
+        <v>70.400000000000006</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="6">
         <f>B5/B3/B11*10000/B7</f>
-        <v>1.4204545454545454</v>
+        <v>1.6233766233766234</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>54</v>
       </c>
       <c r="E17" s="12">
         <f>E13*0.6/(E25*2+E24)</f>
-        <v>2.5599999999999996</v>
+        <v>2.3225806451612905</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>55</v>
@@ -1030,45 +1100,51 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="6">
         <f>ROUNDDOWN(B7/100/(1-B7/100)*B3/(B4+B6),0)</f>
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="5">
+        <v>1400</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
       <c r="H18" s="5">
         <f>E14*E24^2/1000</f>
-        <v>621.52599999999995</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>388.125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="6">
         <f>1/(B8/100*B4)*(B5/B4)*(B7/100)/B12*1000</f>
-        <v>46.296296296296305</v>
+        <v>40.50925925925926</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="H19" s="5">
         <f>E14*E25^2/1000</f>
-        <v>7.2640000000000002</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>5.5890000000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B20" s="8">
         <f xml:space="preserve"> 1/(1+B3/B4/B18)</f>
-        <v>0.375</v>
+        <v>0.32926829268292684</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>22</v>
@@ -1081,16 +1157,16 @@
       </c>
       <c r="H20" s="5">
         <f>E23*E24/1000*E15</f>
-        <v>403.50720000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>272.64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B21" s="8">
         <f>1/(1+B2/B4/B18)</f>
-        <v>0.24812030075187966</v>
+        <v>0.21259842519685038</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>34</v>
@@ -1103,16 +1179,16 @@
       </c>
       <c r="H21" s="5">
         <f>E25*E15*E23/1000</f>
-        <v>43.622399999999999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>32.716800000000006</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="8">
         <f>1/(1+B3/B4/E26)</f>
-        <v>0.33534743202416917</v>
+        <v>0.3125</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>33</v>
@@ -1120,14 +1196,21 @@
       <c r="E22" s="5">
         <v>27.7</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G22" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H22" s="5">
+        <f>(4*3.1415*10^-7*E24^2*E12/H18-(E16*10^-3/(E18)))*1000</f>
+        <v>0.10350108120542902</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="8">
         <f>1/(1+B2/B4/E26)</f>
-        <v>0.2172211350293542</v>
+        <v>0.2</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>32</v>
@@ -1136,31 +1219,31 @@
         <v>51.2</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D24" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E24" s="5">
         <f>ROUNDUP(B2*B21/B12/E12*1000/E11,0)</f>
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D25" s="3" t="s">
         <v>24</v>
       </c>
       <c r="E25" s="5">
         <f>ROUNDUP(E24/B18,0)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D26" s="3" t="s">
         <v>29</v>
       </c>
       <c r="E26" s="6">
         <f>E24/E25</f>
-        <v>9.25</v>
+        <v>8.3333333333333339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>